<commit_message>
Updated the use case sheet
</commit_message>
<xml_diff>
--- a/BarCode/Documents/Use Case.xlsx
+++ b/BarCode/Documents/Use Case.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Use Case" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -473,7 +473,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -483,7 +483,7 @@
     <col min="3" max="20" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>